<commit_message>
add reactor-netty benchmark results
</commit_message>
<xml_diff>
--- a/benchmark-results/results.xlsx
+++ b/benchmark-results/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianjia/workspace-os/api-gateways-comparison/benchmark-results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F02D86-56A9-4A4A-A1FB-58C6DAC3D6D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59D9CAE-43D7-A440-933E-3971D745EE3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17040" activeTab="1" xr2:uid="{A59EA06C-3223-3348-9DE9-0419F281F7CE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,6 +119,10 @@
   </si>
   <si>
     <t>Vert.x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reactor Netty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -329,9 +333,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -345,12 +349,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -358,10 +365,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>17563.793000000001</c:v>
                 </c:pt>
@@ -375,12 +382,15 @@
                   <c:v>16093.133</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>16269.307000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>12431.767</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6063.9210000000003</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>5945.4530000000004</c:v>
                 </c:pt>
               </c:numCache>
@@ -715,9 +725,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -731,12 +741,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -744,10 +757,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$8</c:f>
+              <c:f>Sheet1!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -761,12 +774,15 @@
                   <c:v>0.9162675169309954</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.92629803824265067</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.70780650853719351</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.34525122221606686</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.33850620990579883</c:v>
                 </c:pt>
               </c:numCache>
@@ -1109,9 +1125,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1125,12 +1141,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -1138,10 +1157,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>91</c:v>
                 </c:pt>
@@ -1155,12 +1174,15 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>153</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>275</c:v>
                 </c:pt>
               </c:numCache>
@@ -1254,9 +1276,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1270,12 +1292,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -1283,10 +1308,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>174</c:v>
                 </c:pt>
@@ -1300,12 +1325,15 @@
                   <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>192</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>562</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>486</c:v>
                 </c:pt>
               </c:numCache>
@@ -1399,9 +1427,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1415,12 +1443,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -1428,10 +1459,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>324</c:v>
                 </c:pt>
@@ -1445,12 +1476,15 @@
                   <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>259</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>883</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>581</c:v>
                 </c:pt>
               </c:numCache>
@@ -1544,10 +1578,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$8</c:f>
+              <c:f>Sheet1!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>689</c:v>
                 </c:pt>
@@ -1561,12 +1595,15 @@
                   <c:v>712</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1327</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>636</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1358</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1440</c:v>
                 </c:pt>
               </c:numCache>
@@ -1660,10 +1697,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$8</c:f>
+              <c:f>Sheet1!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1639</c:v>
                 </c:pt>
@@ -1677,12 +1714,15 @@
                   <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>10264</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1369</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1538</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1737</c:v>
                 </c:pt>
               </c:numCache>
@@ -2055,9 +2095,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -2071,12 +2111,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -2084,10 +2127,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$8</c:f>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>102</c:v>
                 </c:pt>
@@ -2101,12 +2144,15 @@
                   <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>303</c:v>
                 </c:pt>
               </c:numCache>
@@ -2448,9 +2494,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -2464,12 +2510,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -2477,10 +2526,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$8</c:f>
+              <c:f>Sheet1!$O$2:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2494,12 +2543,15 @@
                   <c:v>1.0980392156862746</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.088235294117647</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.4215686274509804</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2.892156862745098</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.9705882352941178</c:v>
                 </c:pt>
               </c:numCache>
@@ -2842,9 +2894,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -2858,12 +2910,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -2871,10 +2926,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:f>Sheet1!$J$2:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2888,12 +2943,15 @@
                   <c:v>1.098901098901099</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.90109890109890112</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.6813186813186813</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2.9670329670329672</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3.0219780219780219</c:v>
                 </c:pt>
               </c:numCache>
@@ -2987,9 +3045,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -3003,12 +3061,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -3016,10 +3077,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$8</c:f>
+              <c:f>Sheet1!$K$2:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3033,12 +3094,15 @@
                   <c:v>1.0574712643678161</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.2413793103448276</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.103448275862069</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3.2298850574712645</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.7931034482758621</c:v>
                 </c:pt>
               </c:numCache>
@@ -3132,9 +3196,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -3148,12 +3212,15 @@
                   <c:v>Netty</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Reactor Netty</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Vert.x</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Spring Cloud Gateway</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Zuul2</c:v>
                 </c:pt>
               </c:strCache>
@@ -3161,10 +3228,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$8</c:f>
+              <c:f>Sheet1!$L$2:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3178,12 +3245,15 @@
                   <c:v>1.2191358024691359</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.6419753086419753</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.79938271604938271</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2.7253086419753085</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.7932098765432098</c:v>
                 </c:pt>
               </c:numCache>
@@ -3277,10 +3347,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$8</c:f>
+              <c:f>Sheet1!$M$2:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3294,12 +3364,15 @@
                   <c:v>1.0333817126269957</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.9259796806966618</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.92307692307692313</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.9709724238026125</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.0899854862119014</c:v>
                 </c:pt>
               </c:numCache>
@@ -3393,10 +3466,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$8</c:f>
+              <c:f>Sheet1!$N$2:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3410,12 +3483,15 @@
                   <c:v>2.0744356314826113</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>6.2623550945698598</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.83526540573520436</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.93837705918242831</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.0597925564368518</c:v>
                 </c:pt>
               </c:numCache>
@@ -7418,10 +7494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22A2416-4C49-E64F-9511-EC17A66359B2}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7512,7 +7588,7 @@
         <v>102</v>
       </c>
       <c r="I2" s="3">
-        <f t="shared" ref="I2:I8" si="0">B2/$B$2</f>
+        <f t="shared" ref="I2:I9" si="0">B2/$B$2</f>
         <v>1</v>
       </c>
       <c r="J2" s="3">
@@ -7570,27 +7646,27 @@
         <v>0.94441029907378193</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J3:J8" si="1">C3/$C$2</f>
+        <f t="shared" ref="J3:J9" si="1">C3/$C$2</f>
         <v>0.95604395604395609</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K8" si="2">D3/$D$2</f>
+        <f t="shared" ref="K3:K9" si="2">D3/$D$2</f>
         <v>1.0977011494252873</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L8" si="3">E3/$E$2</f>
+        <f t="shared" ref="L3:L9" si="3">E3/$E$2</f>
         <v>1.3765432098765431</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M8" si="4">F3/$F$2</f>
+        <f t="shared" ref="M3:M9" si="4">F3/$F$2</f>
         <v>1.6531204644412192</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N8" si="5">G3/$G$2</f>
+        <f t="shared" ref="N3:N9" si="5">G3/$G$2</f>
         <v>2.4813910921293472</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" ref="O3:O8" si="6">H3/$H$2</f>
+        <f t="shared" ref="O3:O9" si="6">H3/$H$2</f>
         <v>1.0588235294117647</v>
       </c>
     </row>
@@ -7704,162 +7780,216 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
-        <v>12431.767</v>
+        <v>16269.307000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="E6" s="1">
-        <v>259</v>
+        <v>532</v>
       </c>
       <c r="F6" s="1">
-        <v>636</v>
+        <v>1327</v>
       </c>
       <c r="G6" s="1">
-        <v>1369</v>
+        <v>10264</v>
       </c>
       <c r="H6" s="1">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="I6" s="3">
-        <f t="shared" ref="I6" si="7">B6/$B$2</f>
-        <v>0.70780650853719351</v>
+        <f>B6/$B$2</f>
+        <v>0.92629803824265067</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" ref="J6" si="8">C6/$C$2</f>
-        <v>1.6813186813186813</v>
+        <f t="shared" ref="J6" si="7">C6/$C$2</f>
+        <v>0.90109890109890112</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" ref="K6" si="9">D6/$D$2</f>
-        <v>1.103448275862069</v>
+        <f t="shared" ref="K6" si="8">D6/$D$2</f>
+        <v>1.2413793103448276</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" ref="L6" si="10">E6/$E$2</f>
-        <v>0.79938271604938271</v>
+        <f t="shared" ref="L6" si="9">E6/$E$2</f>
+        <v>1.6419753086419753</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" ref="M6" si="11">F6/$F$2</f>
-        <v>0.92307692307692313</v>
+        <f t="shared" ref="M6" si="10">F6/$F$2</f>
+        <v>1.9259796806966618</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" ref="N6" si="12">G6/$G$2</f>
-        <v>0.83526540573520436</v>
+        <f t="shared" ref="N6" si="11">G6/$G$2</f>
+        <v>6.2623550945698598</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" ref="O6" si="13">H6/$H$2</f>
-        <v>1.4215686274509804</v>
+        <f t="shared" ref="O6" si="12">H6/$H$2</f>
+        <v>1.088235294117647</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
-        <v>6063.9210000000003</v>
+        <v>12431.767</v>
       </c>
       <c r="C7" s="1">
-        <v>270</v>
+        <v>153</v>
       </c>
       <c r="D7" s="1">
-        <v>562</v>
+        <v>192</v>
       </c>
       <c r="E7" s="1">
-        <v>883</v>
+        <v>259</v>
       </c>
       <c r="F7" s="1">
-        <v>1358</v>
+        <v>636</v>
       </c>
       <c r="G7" s="1">
-        <v>1538</v>
+        <v>1369</v>
       </c>
       <c r="H7" s="1">
-        <v>295</v>
+        <v>145</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.34525122221606686</v>
+        <f t="shared" ref="I7" si="13">B7/$B$2</f>
+        <v>0.70780650853719351</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9670329670329672</v>
+        <f t="shared" ref="J7" si="14">C7/$C$2</f>
+        <v>1.6813186813186813</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="2"/>
-        <v>3.2298850574712645</v>
+        <f t="shared" ref="K7" si="15">D7/$D$2</f>
+        <v>1.103448275862069</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="3"/>
-        <v>2.7253086419753085</v>
+        <f t="shared" ref="L7" si="16">E7/$E$2</f>
+        <v>0.79938271604938271</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="4"/>
-        <v>1.9709724238026125</v>
+        <f t="shared" ref="M7" si="17">F7/$F$2</f>
+        <v>0.92307692307692313</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="5"/>
-        <v>0.93837705918242831</v>
+        <f t="shared" ref="N7" si="18">G7/$G$2</f>
+        <v>0.83526540573520436</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="6"/>
-        <v>2.892156862745098</v>
+        <f t="shared" ref="O7" si="19">H7/$H$2</f>
+        <v>1.4215686274509804</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
-        <v>5945.4530000000004</v>
+        <v>6063.9210000000003</v>
       </c>
       <c r="C8" s="1">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D8" s="1">
-        <v>486</v>
+        <v>562</v>
       </c>
       <c r="E8" s="1">
-        <v>581</v>
+        <v>883</v>
       </c>
       <c r="F8" s="1">
-        <v>1440</v>
+        <v>1358</v>
       </c>
       <c r="G8" s="1">
-        <v>1737</v>
+        <v>1538</v>
       </c>
       <c r="H8" s="1">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="0"/>
-        <v>0.33850620990579883</v>
+        <v>0.34525122221606686</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="1"/>
-        <v>3.0219780219780219</v>
+        <v>2.9670329670329672</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" si="2"/>
-        <v>2.7931034482758621</v>
+        <v>3.2298850574712645</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" si="3"/>
-        <v>1.7932098765432098</v>
+        <v>2.7253086419753085</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="4"/>
-        <v>2.0899854862119014</v>
+        <v>1.9709724238026125</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="5"/>
+        <v>0.93837705918242831</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="6"/>
+        <v>2.892156862745098</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5945.4530000000004</v>
+      </c>
+      <c r="C9" s="1">
+        <v>275</v>
+      </c>
+      <c r="D9" s="1">
+        <v>486</v>
+      </c>
+      <c r="E9" s="1">
+        <v>581</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1440</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1737</v>
+      </c>
+      <c r="H9" s="1">
+        <v>303</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33850620990579883</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
+        <v>3.0219780219780219</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="2"/>
+        <v>2.7931034482758621</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="3"/>
+        <v>1.7932098765432098</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="4"/>
+        <v>2.0899854862119014</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="5"/>
         <v>1.0597925564368518</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O9" s="3">
         <f t="shared" si="6"/>
         <v>2.9705882352941178</v>
       </c>
@@ -7874,7 +8004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEDC3A4-9CCE-AD40-A415-782FA5322253}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add: netty-http benchmark result
</commit_message>
<xml_diff>
--- a/benchmark-results/results.xlsx
+++ b/benchmark-results/results.xlsx
@@ -8,20 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianjia/workspace-os/api-gateways-comparison/benchmark-results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCF1BF5-ED10-7B47-878F-2ECF43224CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAE2C01-28FA-2F4A-9E12-12DD16B0A2CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17040" activeTab="1" xr2:uid="{A59EA06C-3223-3348-9DE9-0419F281F7CE}"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="27760" windowHeight="17040" activeTab="1" xr2:uid="{A59EA06C-3223-3348-9DE9-0419F281F7CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$9</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$9</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$2:$A$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$9</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,27 +68,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Haproxy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Netty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nginx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spring Cloud Gateway</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tomcat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zuul2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -126,15 +100,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Vert.x</t>
+    <t>Go(L7)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Reactor Netty</t>
+    <t>Netty(L7)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Go Http</t>
+    <t>Reactor Netty(L4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Netty(L4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nginx(L7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haproxy(L7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vert.x(L7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring Cloud Gateway(L7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zuul2(L7)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -345,45 +343,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>17563.793000000001</c:v>
                 </c:pt>
@@ -397,18 +398,21 @@
                   <c:v>16093.133</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>15543.826999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>16269.307000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>12431.767</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>6063.9210000000003</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>5945.4530000000004</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>5219.5200000000004</c:v>
                 </c:pt>
               </c:numCache>
@@ -743,45 +747,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$10</c:f>
+              <c:f>Sheet1!$I$2:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -795,18 +802,21 @@
                   <c:v>0.9162675169309954</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.8849926095120797</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.92629803824265067</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.70780650853719351</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.34525122221606686</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.33850620990579883</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.29717498947977811</c:v>
                 </c:pt>
               </c:numCache>
@@ -1149,45 +1159,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>91</c:v>
                 </c:pt>
@@ -1201,18 +1214,21 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>153</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>275</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>342</c:v>
                 </c:pt>
               </c:numCache>
@@ -1306,45 +1322,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>174</c:v>
                 </c:pt>
@@ -1358,18 +1377,21 @@
                   <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>216</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>192</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>562</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>563</c:v>
                 </c:pt>
               </c:numCache>
@@ -1463,45 +1485,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$10</c:f>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>324</c:v>
                 </c:pt>
@@ -1515,18 +1540,21 @@
                   <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>532</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>259</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>883</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>581</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>730</c:v>
                 </c:pt>
               </c:numCache>
@@ -1620,45 +1648,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$10</c:f>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>689</c:v>
                 </c:pt>
@@ -1672,18 +1703,21 @@
                   <c:v>712</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1327</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>636</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1358</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1440</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>955</c:v>
                 </c:pt>
               </c:numCache>
@@ -1777,45 +1811,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$10</c:f>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1639</c:v>
                 </c:pt>
@@ -1829,18 +1866,21 @@
                   <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>7483</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>10264</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1369</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1538</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1737</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1646</c:v>
                 </c:pt>
               </c:numCache>
@@ -2213,45 +2253,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$10</c:f>
+              <c:f>Sheet1!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>102</c:v>
                 </c:pt>
@@ -2265,18 +2308,21 @@
                   <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>111</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>295</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>303</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>345</c:v>
                 </c:pt>
               </c:numCache>
@@ -2618,45 +2664,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$10</c:f>
+              <c:f>Sheet1!$O$2:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2670,18 +2719,21 @@
                   <c:v>1.0980392156862746</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.1372549019607843</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.088235294117647</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.4215686274509804</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.892156862745098</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2.9705882352941178</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3.3823529411764706</c:v>
                 </c:pt>
               </c:numCache>
@@ -3024,45 +3076,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$10</c:f>
+              <c:f>Sheet1!$J$2:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3076,18 +3131,21 @@
                   <c:v>1.098901098901099</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.92307692307692313</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.90109890109890112</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.6813186813186813</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.9670329670329672</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3.0219780219780219</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3.7582417582417582</c:v>
                 </c:pt>
               </c:numCache>
@@ -3181,45 +3239,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$10</c:f>
+              <c:f>Sheet1!$K$2:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3233,18 +3294,21 @@
                   <c:v>1.0574712643678161</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.3103448275862069</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.2413793103448276</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.103448275862069</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3.2298850574712645</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2.7931034482758621</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3.235632183908046</c:v>
                 </c:pt>
               </c:numCache>
@@ -3338,45 +3402,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$10</c:f>
+              <c:f>Sheet1!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3390,18 +3457,21 @@
                   <c:v>1.2191358024691359</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.6944444444444444</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.6419753086419753</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.79938271604938271</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.7253086419753085</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1.7932098765432098</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>2.2530864197530862</c:v>
                 </c:pt>
               </c:numCache>
@@ -3495,45 +3565,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$10</c:f>
+              <c:f>Sheet1!$M$2:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3547,18 +3620,21 @@
                   <c:v>1.0333817126269957</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.7532656023222062</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.9259796806966618</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.92307692307692313</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.9709724238026125</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2.0899854862119014</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1.3860667634252539</c:v>
                 </c:pt>
               </c:numCache>
@@ -3652,45 +3728,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Haproxy</c:v>
+                  <c:v>Haproxy(L7)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Nginx</c:v>
+                  <c:v>Nginx(L7)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Netty</c:v>
+                  <c:v>Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Reactor Netty</c:v>
+                  <c:v>Netty(L7)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Vert.x</c:v>
+                  <c:v>Reactor Netty(L4)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Spring Cloud Gateway</c:v>
+                  <c:v>Vert.x(L7)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Zuul2</c:v>
+                  <c:v>Spring Cloud Gateway(L7)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Go Http</c:v>
+                  <c:v>Zuul2(L7)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$10</c:f>
+              <c:f>Sheet1!$N$2:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3704,18 +3783,21 @@
                   <c:v>2.0744356314826113</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>4.5655887736424647</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6.2623550945698598</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.83526540573520436</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.93837705918242831</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1.0597925564368518</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1.0042708968883465</c:v>
                 </c:pt>
               </c:numCache>
@@ -7198,8 +7280,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7236,8 +7318,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7312,8 +7394,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7350,8 +7432,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7388,8 +7470,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7718,10 +7800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22A2416-4C49-E64F-9511-EC17A66359B2}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9:O10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7765,30 +7847,30 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>17563.793000000001</v>
@@ -7812,7 +7894,7 @@
         <v>102</v>
       </c>
       <c r="I2" s="3">
-        <f t="shared" ref="I2:I10" si="0">B2/$B$2</f>
+        <f t="shared" ref="I2:I11" si="0">B2/$B$2</f>
         <v>1</v>
       </c>
       <c r="J2" s="3">
@@ -7842,7 +7924,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>16587.427</v>
@@ -7870,33 +7952,33 @@
         <v>0.94441029907378193</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J3:J10" si="1">C3/$C$2</f>
+        <f t="shared" ref="J3:J11" si="1">C3/$C$2</f>
         <v>0.95604395604395609</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K10" si="2">D3/$D$2</f>
+        <f t="shared" ref="K3:K11" si="2">D3/$D$2</f>
         <v>1.0977011494252873</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L10" si="3">E3/$E$2</f>
+        <f t="shared" ref="L3:L11" si="3">E3/$E$2</f>
         <v>1.3765432098765431</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M10" si="4">F3/$F$2</f>
+        <f t="shared" ref="M3:M11" si="4">F3/$F$2</f>
         <v>1.6531204644412192</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N10" si="5">G3/$G$2</f>
+        <f t="shared" ref="N3:N11" si="5">G3/$G$2</f>
         <v>2.4813910921293472</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" ref="O3:O10" si="6">H3/$H$2</f>
+        <f t="shared" ref="O3:O11" si="6">H3/$H$2</f>
         <v>1.0588235294117647</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>16125.331</v>
@@ -7950,7 +8032,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>16093.133</v>
@@ -8004,270 +8086,324 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
-        <v>16269.307000000001</v>
+        <v>15543.826999999999</v>
       </c>
       <c r="C6" s="1">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="E6" s="1">
-        <v>532</v>
+        <v>549</v>
       </c>
       <c r="F6" s="1">
-        <v>1327</v>
+        <v>1208</v>
       </c>
       <c r="G6" s="1">
-        <v>10264</v>
+        <v>7483</v>
       </c>
       <c r="H6" s="1">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="I6" s="3">
-        <f>B6/$B$2</f>
-        <v>0.92629803824265067</v>
+        <f t="shared" ref="I6" si="7">B6/$B$2</f>
+        <v>0.8849926095120797</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" ref="J6" si="7">C6/$C$2</f>
-        <v>0.90109890109890112</v>
+        <f t="shared" ref="J6" si="8">C6/$C$2</f>
+        <v>0.92307692307692313</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" ref="K6" si="8">D6/$D$2</f>
-        <v>1.2413793103448276</v>
+        <f t="shared" ref="K6" si="9">D6/$D$2</f>
+        <v>1.3103448275862069</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" ref="L6" si="9">E6/$E$2</f>
-        <v>1.6419753086419753</v>
+        <f t="shared" ref="L6" si="10">E6/$E$2</f>
+        <v>1.6944444444444444</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" ref="M6" si="10">F6/$F$2</f>
-        <v>1.9259796806966618</v>
+        <f t="shared" ref="M6" si="11">F6/$F$2</f>
+        <v>1.7532656023222062</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" ref="N6" si="11">G6/$G$2</f>
-        <v>6.2623550945698598</v>
+        <f t="shared" ref="N6" si="12">G6/$G$2</f>
+        <v>4.5655887736424647</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" ref="O6" si="12">H6/$H$2</f>
-        <v>1.088235294117647</v>
+        <f t="shared" ref="O6" si="13">H6/$H$2</f>
+        <v>1.1372549019607843</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>12431.767</v>
+        <v>16269.307000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="E7" s="1">
-        <v>259</v>
+        <v>532</v>
       </c>
       <c r="F7" s="1">
-        <v>636</v>
+        <v>1327</v>
       </c>
       <c r="G7" s="1">
-        <v>1369</v>
+        <v>10264</v>
       </c>
       <c r="H7" s="1">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" ref="I7" si="13">B7/$B$2</f>
-        <v>0.70780650853719351</v>
+        <f>B7/$B$2</f>
+        <v>0.92629803824265067</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ref="J7" si="14">C7/$C$2</f>
-        <v>1.6813186813186813</v>
+        <v>0.90109890109890112</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" ref="K7" si="15">D7/$D$2</f>
-        <v>1.103448275862069</v>
+        <v>1.2413793103448276</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" ref="L7" si="16">E7/$E$2</f>
-        <v>0.79938271604938271</v>
+        <v>1.6419753086419753</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" ref="M7" si="17">F7/$F$2</f>
-        <v>0.92307692307692313</v>
+        <v>1.9259796806966618</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" ref="N7" si="18">G7/$G$2</f>
-        <v>0.83526540573520436</v>
+        <v>6.2623550945698598</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" ref="O7" si="19">H7/$H$2</f>
-        <v>1.4215686274509804</v>
+        <v>1.088235294117647</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
-        <v>6063.9210000000003</v>
+        <v>12431.767</v>
       </c>
       <c r="C8" s="1">
-        <v>270</v>
+        <v>153</v>
       </c>
       <c r="D8" s="1">
-        <v>562</v>
+        <v>192</v>
       </c>
       <c r="E8" s="1">
-        <v>883</v>
+        <v>259</v>
       </c>
       <c r="F8" s="1">
-        <v>1358</v>
+        <v>636</v>
       </c>
       <c r="G8" s="1">
-        <v>1538</v>
+        <v>1369</v>
       </c>
       <c r="H8" s="1">
-        <v>295</v>
+        <v>145</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.34525122221606686</v>
+        <f t="shared" ref="I8" si="20">B8/$B$2</f>
+        <v>0.70780650853719351</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9670329670329672</v>
+        <f t="shared" ref="J8" si="21">C8/$C$2</f>
+        <v>1.6813186813186813</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="2"/>
-        <v>3.2298850574712645</v>
+        <f t="shared" ref="K8" si="22">D8/$D$2</f>
+        <v>1.103448275862069</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="3"/>
-        <v>2.7253086419753085</v>
+        <f t="shared" ref="L8" si="23">E8/$E$2</f>
+        <v>0.79938271604938271</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="4"/>
-        <v>1.9709724238026125</v>
+        <f t="shared" ref="M8" si="24">F8/$F$2</f>
+        <v>0.92307692307692313</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="5"/>
-        <v>0.93837705918242831</v>
+        <f t="shared" ref="N8" si="25">G8/$G$2</f>
+        <v>0.83526540573520436</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="6"/>
-        <v>2.892156862745098</v>
+        <f t="shared" ref="O8" si="26">H8/$H$2</f>
+        <v>1.4215686274509804</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
-        <v>5945.4530000000004</v>
+        <v>6063.9210000000003</v>
       </c>
       <c r="C9" s="1">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D9" s="1">
-        <v>486</v>
+        <v>562</v>
       </c>
       <c r="E9" s="1">
-        <v>581</v>
+        <v>883</v>
       </c>
       <c r="F9" s="1">
-        <v>1440</v>
+        <v>1358</v>
       </c>
       <c r="G9" s="1">
-        <v>1737</v>
+        <v>1538</v>
       </c>
       <c r="H9" s="1">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>0.33850620990579883</v>
+        <v>0.34525122221606686</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="1"/>
-        <v>3.0219780219780219</v>
+        <v>2.9670329670329672</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="2"/>
-        <v>2.7931034482758621</v>
+        <v>3.2298850574712645</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" si="3"/>
-        <v>1.7932098765432098</v>
+        <v>2.7253086419753085</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="4"/>
-        <v>2.0899854862119014</v>
+        <v>1.9709724238026125</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="5"/>
-        <v>1.0597925564368518</v>
+        <v>0.93837705918242831</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="6"/>
-        <v>2.9705882352941178</v>
+        <v>2.892156862745098</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1">
-        <v>5219.5200000000004</v>
+        <v>5945.4530000000004</v>
       </c>
       <c r="C10" s="1">
-        <v>342</v>
+        <v>275</v>
       </c>
       <c r="D10" s="1">
-        <v>563</v>
+        <v>486</v>
       </c>
       <c r="E10" s="1">
-        <v>730</v>
+        <v>581</v>
       </c>
       <c r="F10" s="1">
-        <v>955</v>
+        <v>1440</v>
       </c>
       <c r="G10" s="1">
-        <v>1646</v>
+        <v>1737</v>
       </c>
       <c r="H10" s="1">
-        <v>345</v>
+        <v>303</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>0.29717498947977811</v>
+        <v>0.33850620990579883</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="1"/>
-        <v>3.7582417582417582</v>
+        <v>3.0219780219780219</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="2"/>
-        <v>3.235632183908046</v>
+        <v>2.7931034482758621</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" si="3"/>
-        <v>2.2530864197530862</v>
+        <v>1.7932098765432098</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="4"/>
-        <v>1.3860667634252539</v>
+        <v>2.0899854862119014</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="5"/>
+        <v>1.0597925564368518</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="6"/>
+        <v>2.9705882352941178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5219.5200000000004</v>
+      </c>
+      <c r="C11" s="1">
+        <v>342</v>
+      </c>
+      <c r="D11" s="1">
+        <v>563</v>
+      </c>
+      <c r="E11" s="1">
+        <v>730</v>
+      </c>
+      <c r="F11" s="1">
+        <v>955</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1646</v>
+      </c>
+      <c r="H11" s="1">
+        <v>345</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.29717498947977811</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7582417582417582</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="2"/>
+        <v>3.235632183908046</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="3"/>
+        <v>2.2530864197530862</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="4"/>
+        <v>1.3860667634252539</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="5"/>
         <v>1.0042708968883465</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O11" s="3">
         <f t="shared" si="6"/>
         <v>3.3823529411764706</v>
       </c>
@@ -8282,7 +8418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEDC3A4-9CCE-AD40-A415-782FA5322253}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update: go fasthttp doc and benchmark results
</commit_message>
<xml_diff>
--- a/benchmark-results/results.xlsx
+++ b/benchmark-results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianjia/workspace-os/api-gateways-comparison/benchmark-results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAE2C01-28FA-2F4A-9E12-12DD16B0A2CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59B8377-6591-EA42-8859-ECD432C1CBF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="27760" windowHeight="17040" activeTab="1" xr2:uid="{A59EA06C-3223-3348-9DE9-0419F281F7CE}"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17040" activeTab="1" xr2:uid="{A59EA06C-3223-3348-9DE9-0419F281F7CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Go(L7)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Netty(L7)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -133,6 +129,14 @@
   </si>
   <si>
     <t>Zuul2(L7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoHttp(L7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoFastHttp(L7)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -343,9 +347,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -374,17 +378,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>17563.793000000001</c:v>
                 </c:pt>
@@ -414,6 +421,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5219.5200000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17322.867999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,9 +757,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -778,17 +788,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:f>Sheet1!$I$2:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -818,6 +831,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.29717498947977811</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98628286042769897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1159,9 +1175,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1190,17 +1206,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>91</c:v>
                 </c:pt>
@@ -1230,6 +1249,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,9 +1344,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1353,17 +1375,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>174</c:v>
                 </c:pt>
@@ -1393,6 +1418,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1485,9 +1513,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1516,17 +1544,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>324</c:v>
                 </c:pt>
@@ -1556,6 +1587,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1648,9 +1682,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1679,17 +1713,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:f>Sheet1!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>689</c:v>
                 </c:pt>
@@ -1719,6 +1756,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>955</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1811,9 +1851,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -1842,17 +1882,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$11</c:f>
+              <c:f>Sheet1!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1639</c:v>
                 </c:pt>
@@ -1882,6 +1925,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1646</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3936</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2253,9 +2299,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -2284,17 +2330,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:f>Sheet1!$H$2:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>102</c:v>
                 </c:pt>
@@ -2324,6 +2373,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2664,9 +2716,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -2695,17 +2747,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$11</c:f>
+              <c:f>Sheet1!$O$2:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2735,6 +2790,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.3823529411764706</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0098039215686274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3076,9 +3134,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -3107,17 +3165,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$11</c:f>
+              <c:f>Sheet1!$J$2:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3147,6 +3208,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.7582417582417582</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94505494505494503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3239,9 +3303,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -3270,17 +3334,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$11</c:f>
+              <c:f>Sheet1!$K$2:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3310,6 +3377,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.235632183908046</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0172413793103448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3402,9 +3472,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -3433,17 +3503,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$11</c:f>
+              <c:f>Sheet1!$L$2:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3473,6 +3546,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.2530864197530862</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3565,9 +3641,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -3596,17 +3672,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$11</c:f>
+              <c:f>Sheet1!$M$2:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3636,6 +3715,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.3860667634252539</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.637155297532656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3728,9 +3810,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Tomcat</c:v>
                 </c:pt>
@@ -3759,17 +3841,20 @@
                   <c:v>Zuul2(L7)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Go(L7)</c:v>
+                  <c:v>GoHttp(L7)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>GoFastHttp(L7)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$11</c:f>
+              <c:f>Sheet1!$N$2:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3799,6 +3884,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.0042708968883465</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.4014643075045758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7280,8 +7368,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7312,14 +7400,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7357,7 +7445,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7394,8 +7482,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7426,14 +7514,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7464,14 +7552,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -7800,10 +7888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22A2416-4C49-E64F-9511-EC17A66359B2}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7894,7 +7982,7 @@
         <v>102</v>
       </c>
       <c r="I2" s="3">
-        <f t="shared" ref="I2:I11" si="0">B2/$B$2</f>
+        <f t="shared" ref="I2:I12" si="0">B2/$B$2</f>
         <v>1</v>
       </c>
       <c r="J2" s="3">
@@ -7924,7 +8012,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>16587.427</v>
@@ -7952,33 +8040,33 @@
         <v>0.94441029907378193</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J3:J11" si="1">C3/$C$2</f>
+        <f t="shared" ref="J3:J12" si="1">C3/$C$2</f>
         <v>0.95604395604395609</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K11" si="2">D3/$D$2</f>
+        <f t="shared" ref="K3:K12" si="2">D3/$D$2</f>
         <v>1.0977011494252873</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L11" si="3">E3/$E$2</f>
+        <f t="shared" ref="L3:L12" si="3">E3/$E$2</f>
         <v>1.3765432098765431</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M11" si="4">F3/$F$2</f>
+        <f t="shared" ref="M3:M12" si="4">F3/$F$2</f>
         <v>1.6531204644412192</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N11" si="5">G3/$G$2</f>
+        <f t="shared" ref="N3:N12" si="5">G3/$G$2</f>
         <v>2.4813910921293472</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" ref="O3:O11" si="6">H3/$H$2</f>
+        <f t="shared" ref="O3:O12" si="6">H3/$H$2</f>
         <v>1.0588235294117647</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>16125.331</v>
@@ -8032,7 +8120,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>16093.133</v>
@@ -8086,7 +8174,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>15543.826999999999</v>
@@ -8140,7 +8228,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>16269.307000000001</v>
@@ -8194,7 +8282,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>12431.767</v>
@@ -8248,7 +8336,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>6063.9210000000003</v>
@@ -8302,7 +8390,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1">
         <v>5945.4530000000004</v>
@@ -8356,7 +8444,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>5219.5200000000004</v>
@@ -8380,32 +8468,86 @@
         <v>345</v>
       </c>
       <c r="I11" s="3">
+        <f t="shared" ref="I11" si="27">B11/$B$2</f>
+        <v>0.29717498947977811</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" ref="J11" si="28">C11/$C$2</f>
+        <v>3.7582417582417582</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" ref="K11" si="29">D11/$D$2</f>
+        <v>3.235632183908046</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" ref="L11" si="30">E11/$E$2</f>
+        <v>2.2530864197530862</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" ref="M11" si="31">F11/$F$2</f>
+        <v>1.3860667634252539</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" ref="N11" si="32">G11/$G$2</f>
+        <v>1.0042708968883465</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" ref="O11" si="33">H11/$H$2</f>
+        <v>3.3823529411764706</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
+        <v>17322.867999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>86</v>
+      </c>
+      <c r="D12" s="1">
+        <v>177</v>
+      </c>
+      <c r="E12" s="1">
+        <v>378</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1128</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3936</v>
+      </c>
+      <c r="H12" s="1">
+        <v>103</v>
+      </c>
+      <c r="I12" s="3">
         <f t="shared" si="0"/>
-        <v>0.29717498947977811</v>
-      </c>
-      <c r="J11" s="3">
+        <v>0.98628286042769897</v>
+      </c>
+      <c r="J12" s="3">
         <f t="shared" si="1"/>
-        <v>3.7582417582417582</v>
-      </c>
-      <c r="K11" s="3">
+        <v>0.94505494505494503</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="2"/>
-        <v>3.235632183908046</v>
-      </c>
-      <c r="L11" s="3">
+        <v>1.0172413793103448</v>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" si="3"/>
-        <v>2.2530864197530862</v>
-      </c>
-      <c r="M11" s="3">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="M12" s="3">
         <f t="shared" si="4"/>
-        <v>1.3860667634252539</v>
-      </c>
-      <c r="N11" s="3">
+        <v>1.637155297532656</v>
+      </c>
+      <c r="N12" s="3">
         <f t="shared" si="5"/>
-        <v>1.0042708968883465</v>
-      </c>
-      <c r="O11" s="3">
+        <v>2.4014643075045758</v>
+      </c>
+      <c r="O12" s="3">
         <f t="shared" si="6"/>
-        <v>3.3823529411764706</v>
+        <v>1.0098039215686274</v>
       </c>
     </row>
   </sheetData>
@@ -8418,8 +8560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEDC3A4-9CCE-AD40-A415-782FA5322253}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="X53" sqref="X53"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>